<commit_message>
Dec 2023 update 1
</commit_message>
<xml_diff>
--- a/Practical_classes/Week9_student_project_initiation/tasks_people.xlsx
+++ b/Practical_classes/Week9_student_project_initiation/tasks_people.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keil\Dropbox\GitHub\Spatial-Ecology-and-Macroecology\Practical_classes\Week9_student_project_initiation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936CAB0A-938F-43EF-9EF3-924C47808269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5425BE1D-0196-47EA-8082-BF2379DA9146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Coufal</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Lama guanicoe</t>
   </si>
   <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
     <t>Ursus arctus</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Are env. Predictors of the distribution same in Europe vs US?</t>
   </si>
   <si>
-    <t>Are the predictors good for the distribution of V. berus?</t>
-  </si>
-  <si>
     <t>elevation, precipitation, aspect, temperature</t>
   </si>
   <si>
@@ -190,6 +184,67 @@
   </si>
   <si>
     <t>SDM of Lama in two time periods in Argentina, and compare 2010 and 2020</t>
+  </si>
+  <si>
+    <t>Statistical analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presence/pseudo-absence GLM </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Are the predictors good for the distribution of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>V. berus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>MaxEnt</t>
+  </si>
+  <si>
+    <t>How does # of species develop through time, and how does it depend on some simulation parameters?</t>
+  </si>
+  <si>
+    <t>Graphical illustration</t>
+  </si>
+  <si>
+    <t>abundance Poisson GLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxEnt </t>
+  </si>
+  <si>
+    <t>Species richness of mammals</t>
+  </si>
+  <si>
+    <t>linear or poisson regression</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -536,37 +591,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="57.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="86.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="57.5546875" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,16 +636,19 @@
         <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -597,36 +659,42 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -636,8 +704,14 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -648,16 +722,16 @@
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -668,16 +742,19 @@
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -688,24 +765,42 @@
         <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -713,7 +808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -724,16 +819,19 @@
         <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -744,12 +842,15 @@
         <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>